<commit_message>
transaction upload screen code updated
</commit_message>
<xml_diff>
--- a/docs/security_name.xlsx
+++ b/docs/security_name.xlsx
@@ -1,14 +1,14 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="29426"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="29530"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="F:\helios work\Race2cloud-app\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="F:\helios work\PMS\docs\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="8_{A95969F5-FBC6-461F-84A3-6AFE48F843CE}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{3728DB05-5184-429E-AD72-A7F28332E23C}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12456" xr2:uid="{DDD089E3-2D95-4E70-9E42-43B00B738859}"/>
   </bookViews>
@@ -25,7 +25,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="2055" uniqueCount="2047">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="2064" uniqueCount="2052">
   <si>
     <t>ISIN</t>
   </si>
@@ -6166,6 +6166,21 @@
   </si>
   <si>
     <t>CL Educate Ltd</t>
+  </si>
+  <si>
+    <t>Onmobile Global Ltd</t>
+  </si>
+  <si>
+    <t>INE345A01011</t>
+  </si>
+  <si>
+    <t>HINDOILEXP</t>
+  </si>
+  <si>
+    <t>Hindustan Oil Exploration Company Ltd</t>
+  </si>
+  <si>
+    <t>IRM Energy Ltd</t>
   </si>
 </sst>
 </file>
@@ -6527,16 +6542,16 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{F92EDFD8-4B14-48B0-AC1D-FD5F50E72D2E}">
-  <dimension ref="A1:C718"/>
+  <dimension ref="A1:C721"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="E11" sqref="E11"/>
+      <selection activeCell="D11" sqref="D11"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <cols>
-    <col min="1" max="1" width="10.44140625" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="11.44140625" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="13.33203125" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="13.21875" bestFit="1" customWidth="1"/>
     <col min="3" max="3" width="62.21875" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
@@ -14430,6 +14445,39 @@
         <v>2046</v>
       </c>
     </row>
+    <row r="719" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A719" t="s">
+        <v>1302</v>
+      </c>
+      <c r="B719" t="s">
+        <v>1303</v>
+      </c>
+      <c r="C719" t="s">
+        <v>2047</v>
+      </c>
+    </row>
+    <row r="720" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A720" t="s">
+        <v>2048</v>
+      </c>
+      <c r="B720" t="s">
+        <v>2049</v>
+      </c>
+      <c r="C720" t="s">
+        <v>2050</v>
+      </c>
+    </row>
+    <row r="721" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A721" t="s">
+        <v>1857</v>
+      </c>
+      <c r="B721" t="s">
+        <v>1858</v>
+      </c>
+      <c r="C721" t="s">
+        <v>2051</v>
+      </c>
+    </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>

</xml_diff>